<commit_message>
add Time garden and moving plan
</commit_message>
<xml_diff>
--- a/HabitList.xlsx
+++ b/HabitList.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kan63697\OneDrive\문서\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\03_doc\01_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_FA3482FFA3ED62913A26585E378EBD54CC9F7EFA" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{2FF3D531-8960-406C-AB4D-30FA6D07B8C0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,7 +56,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,6 +329,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -338,12 +343,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -624,7 +623,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -639,14 +638,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="16"/>
+      <c r="A1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:8" ht="33" x14ac:dyDescent="0.3">
@@ -686,7 +685,7 @@
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="17">
+      <c r="A6" s="14">
         <v>1</v>
       </c>
       <c r="B6" s="2"/>
@@ -698,7 +697,7 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="17">
+      <c r="A7" s="14">
         <v>2</v>
       </c>
       <c r="B7" s="2"/>
@@ -710,7 +709,7 @@
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="17">
+      <c r="A8" s="14">
         <v>3</v>
       </c>
       <c r="B8" s="2"/>
@@ -722,7 +721,7 @@
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="17">
+      <c r="A9" s="14">
         <v>4</v>
       </c>
       <c r="B9" s="2"/>
@@ -734,7 +733,7 @@
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="17">
+      <c r="A10" s="14">
         <v>5</v>
       </c>
       <c r="B10" s="2"/>
@@ -746,7 +745,7 @@
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="17">
+      <c r="A11" s="14">
         <v>6</v>
       </c>
       <c r="B11" s="2"/>
@@ -758,7 +757,7 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="17">
+      <c r="A12" s="14">
         <v>7</v>
       </c>
       <c r="B12" s="2"/>
@@ -770,7 +769,7 @@
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="17">
+      <c r="A13" s="14">
         <v>8</v>
       </c>
       <c r="B13" s="2"/>
@@ -782,7 +781,7 @@
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="17">
+      <c r="A14" s="14">
         <v>9</v>
       </c>
       <c r="B14" s="2"/>
@@ -794,7 +793,7 @@
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="17">
+      <c r="A15" s="14">
         <v>10</v>
       </c>
       <c r="B15" s="2"/>
@@ -806,7 +805,7 @@
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="17">
+      <c r="A16" s="14">
         <v>11</v>
       </c>
       <c r="B16" s="2"/>
@@ -818,7 +817,7 @@
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="17">
+      <c r="A17" s="14">
         <v>12</v>
       </c>
       <c r="B17" s="2"/>
@@ -830,7 +829,7 @@
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="17">
+      <c r="A18" s="14">
         <v>13</v>
       </c>
       <c r="B18" s="2"/>
@@ -842,7 +841,7 @@
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="17">
+      <c r="A19" s="14">
         <v>14</v>
       </c>
       <c r="B19" s="2"/>
@@ -854,7 +853,7 @@
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="17">
+      <c r="A20" s="14">
         <v>15</v>
       </c>
       <c r="B20" s="2"/>
@@ -866,7 +865,7 @@
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="17">
+      <c r="A21" s="14">
         <v>16</v>
       </c>
       <c r="B21" s="2"/>
@@ -878,7 +877,7 @@
       <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="17">
+      <c r="A22" s="14">
         <v>17</v>
       </c>
       <c r="B22" s="2"/>
@@ -890,7 +889,7 @@
       <c r="H22" s="7"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="17">
+      <c r="A23" s="14">
         <v>18</v>
       </c>
       <c r="B23" s="2"/>
@@ -902,7 +901,7 @@
       <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="17">
+      <c r="A24" s="14">
         <v>19</v>
       </c>
       <c r="B24" s="2"/>
@@ -914,7 +913,7 @@
       <c r="H24" s="7"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="17">
+      <c r="A25" s="14">
         <v>20</v>
       </c>
       <c r="B25" s="2"/>
@@ -926,7 +925,7 @@
       <c r="H25" s="7"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="17">
+      <c r="A26" s="14">
         <v>21</v>
       </c>
       <c r="B26" s="2"/>
@@ -938,7 +937,7 @@
       <c r="H26" s="7"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="17">
+      <c r="A27" s="14">
         <v>22</v>
       </c>
       <c r="B27" s="2"/>
@@ -950,7 +949,7 @@
       <c r="H27" s="7"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="17">
+      <c r="A28" s="14">
         <v>23</v>
       </c>
       <c r="B28" s="2"/>
@@ -962,7 +961,7 @@
       <c r="H28" s="7"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="17">
+      <c r="A29" s="14">
         <v>24</v>
       </c>
       <c r="B29" s="2"/>
@@ -974,7 +973,7 @@
       <c r="H29" s="7"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="17">
+      <c r="A30" s="14">
         <v>25</v>
       </c>
       <c r="B30" s="2"/>
@@ -986,7 +985,7 @@
       <c r="H30" s="7"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="17">
+      <c r="A31" s="14">
         <v>26</v>
       </c>
       <c r="B31" s="2"/>
@@ -998,7 +997,7 @@
       <c r="H31" s="7"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="17">
+      <c r="A32" s="14">
         <v>27</v>
       </c>
       <c r="B32" s="2"/>
@@ -1010,7 +1009,7 @@
       <c r="H32" s="7"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="17">
+      <c r="A33" s="14">
         <v>28</v>
       </c>
       <c r="B33" s="2"/>
@@ -1022,7 +1021,7 @@
       <c r="H33" s="7"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="17">
+      <c r="A34" s="14">
         <v>29</v>
       </c>
       <c r="B34" s="2"/>
@@ -1034,7 +1033,7 @@
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="17">
+      <c r="A35" s="14">
         <v>30</v>
       </c>
       <c r="B35" s="2"/>
@@ -1046,7 +1045,7 @@
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="18">
+      <c r="A36" s="15">
         <v>31</v>
       </c>
       <c r="B36" s="10"/>

</xml_diff>